<commit_message>
feat: Implement single appointment sheet functionality and update environment variables
</commit_message>
<xml_diff>
--- a/CareDesk/appointments.xlsx
+++ b/CareDesk/appointments.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="2026-01-25" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="2026-01-22" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Appointments" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,87 +413,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Logged At</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Action</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Patient Name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Patient Age or DOB</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Phone</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Department or Doctor</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Reason</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Preferred Date</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Preferred Time</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Visit Type</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Existing Appointment</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -568,12 +486,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-20 17:07:12</t>
+          <t>2026-01-21 16:39:57</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>reschedule</t>
+          <t>book</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -583,12 +501,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>22 (DOB: 1999-01-20)</t>
+          <t>22</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>01518307651</t>
+          <t>0158307641</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -598,61 +516,64 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>low back pain</t>
+          <t>broke hand</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>morning</t>
+          <t>evening</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>first visit</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>2026-01-25 morning</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-20 17:12:36</t>
+          <t>2026-01-21 16:43:17</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>reschedule</t>
+          <t>book</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Hassan</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
+          <t>Sunny</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>01518307651</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
+          <t>01725292621</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>child specialist</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>low back pain</t>
+          <t>fever and cold</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -660,7 +581,11 @@
           <t>morning</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>first visit</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
feat: Add call transfer functionality and update dependencies in CareDesk bot
</commit_message>
<xml_diff>
--- a/CareDesk/appointments.xlsx
+++ b/CareDesk/appointments.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,7 +491,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>book</t>
+          <t>reschedule</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -511,7 +511,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>orthopedics</t>
+          <t>Miss Khalil, orthopedics</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -521,17 +521,22 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2020-02-20</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>evening</t>
+          <t>morning</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>first visit</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2026-01-21 evening</t>
         </is>
       </c>
     </row>
@@ -543,51 +548,108 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>reschedule</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Sunny</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>01725292621</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>child specialist</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>fever and cold</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>evening</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>first visit</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2026-01-21 morning</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-01-21 17:37:10</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>book</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Sunny</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>01725292621</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>child specialist</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>fever and cold</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2026-01-21</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>morning</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Manju</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>01518307641</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Dr. Rachel Morgan, Family Medicine</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>cold issue</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>9 AM</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>first visit</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>